<commit_message>
air blades. air input, ch4, add
</commit_message>
<xml_diff>
--- a/ExcelData/table.xlsx
+++ b/ExcelData/table.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NULS\Desktop\folder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NULS\Desktop\StarAutomation\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1845315A-2460-4F3B-B393-74DD54FA11CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0697C66F-6DE4-499A-9B1A-6E4A187FFCCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="7545" yWindow="3165" windowWidth="17700" windowHeight="11010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28815" yWindow="1290" windowWidth="21135" windowHeight="11220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="85">
   <si>
     <t>Ядро запуска задачи</t>
   </si>
@@ -241,12 +241,129 @@
   <si>
     <t>L3 (29,6)</t>
   </si>
+  <si>
+    <t>78.5</t>
+  </si>
+  <si>
+    <t>79.5</t>
+  </si>
+  <si>
+    <t>78.6</t>
+  </si>
+  <si>
+    <t>79.6</t>
+  </si>
+  <si>
+    <t>78.7</t>
+  </si>
+  <si>
+    <t>79.7</t>
+  </si>
+  <si>
+    <t>78.8</t>
+  </si>
+  <si>
+    <t>79.8</t>
+  </si>
+  <si>
+    <t>78.9</t>
+  </si>
+  <si>
+    <t>79.9</t>
+  </si>
+  <si>
+    <t>78.10</t>
+  </si>
+  <si>
+    <t>79.10</t>
+  </si>
+  <si>
+    <t>78.11</t>
+  </si>
+  <si>
+    <t>30.23</t>
+  </si>
+  <si>
+    <t>31.30</t>
+  </si>
+  <si>
+    <t>30.24</t>
+  </si>
+  <si>
+    <t>31.31</t>
+  </si>
+  <si>
+    <t>30.25</t>
+  </si>
+  <si>
+    <t>31.32</t>
+  </si>
+  <si>
+    <t>30.26</t>
+  </si>
+  <si>
+    <t>31.33</t>
+  </si>
+  <si>
+    <t>30.27</t>
+  </si>
+  <si>
+    <t>31.34</t>
+  </si>
+  <si>
+    <t>30.28</t>
+  </si>
+  <si>
+    <t>31.35</t>
+  </si>
+  <si>
+    <t>30.29</t>
+  </si>
+  <si>
+    <t>0.773</t>
+  </si>
+  <si>
+    <t>0.833</t>
+  </si>
+  <si>
+    <t>0.893</t>
+  </si>
+  <si>
+    <t>0.953</t>
+  </si>
+  <si>
+    <t>0.1013</t>
+  </si>
+  <si>
+    <t>0.1073</t>
+  </si>
+  <si>
+    <t>0.1133</t>
+  </si>
+  <si>
+    <t>0.1193</t>
+  </si>
+  <si>
+    <t>0.1253</t>
+  </si>
+  <si>
+    <t>0.1313</t>
+  </si>
+  <si>
+    <t>0.1373</t>
+  </si>
+  <si>
+    <t>0.1433</t>
+  </si>
+  <si>
+    <t>0.1493</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -269,6 +386,13 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="204"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -808,8 +932,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="E4:Z20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L7" workbookViewId="0">
-      <selection activeCell="T14" sqref="T14"/>
+    <sheetView tabSelected="1" topLeftCell="I7" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1010,13 +1134,13 @@
         <v>12</v>
       </c>
       <c r="P8" s="3" t="s">
-        <v>12</v>
+        <v>46</v>
       </c>
       <c r="Q8" s="3" t="s">
-        <v>12</v>
+        <v>59</v>
       </c>
       <c r="R8" s="3" t="s">
-        <v>12</v>
+        <v>72</v>
       </c>
       <c r="S8" s="3" t="s">
         <v>12</v>
@@ -1070,13 +1194,13 @@
         <v>12</v>
       </c>
       <c r="P9" s="3" t="s">
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="Q9" s="3" t="s">
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="R9" s="3" t="s">
-        <v>12</v>
+        <v>73</v>
       </c>
       <c r="S9" s="3" t="s">
         <v>12</v>
@@ -1130,13 +1254,13 @@
         <v>12</v>
       </c>
       <c r="P10" s="3" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="Q10" s="3" t="s">
-        <v>12</v>
+        <v>61</v>
       </c>
       <c r="R10" s="3" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
       <c r="S10" s="3" t="s">
         <v>12</v>
@@ -1190,13 +1314,13 @@
         <v>12</v>
       </c>
       <c r="P11" s="3" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="Q11" s="3" t="s">
-        <v>12</v>
+        <v>62</v>
       </c>
       <c r="R11" s="3" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="S11" s="3" t="s">
         <v>12</v>
@@ -1250,13 +1374,13 @@
         <v>12</v>
       </c>
       <c r="P12" s="3" t="s">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="Q12" s="3" t="s">
-        <v>12</v>
+        <v>63</v>
       </c>
       <c r="R12" s="3" t="s">
-        <v>12</v>
+        <v>76</v>
       </c>
       <c r="S12" s="3" t="s">
         <v>12</v>
@@ -1310,13 +1434,13 @@
         <v>12</v>
       </c>
       <c r="P13" s="3" t="s">
-        <v>12</v>
+        <v>51</v>
       </c>
       <c r="Q13" s="3" t="s">
-        <v>12</v>
+        <v>64</v>
       </c>
       <c r="R13" s="3" t="s">
-        <v>12</v>
+        <v>77</v>
       </c>
       <c r="S13" s="3" t="s">
         <v>12</v>
@@ -1370,13 +1494,13 @@
         <v>12</v>
       </c>
       <c r="P14" s="3" t="s">
-        <v>12</v>
+        <v>52</v>
       </c>
       <c r="Q14" s="3" t="s">
-        <v>12</v>
+        <v>65</v>
       </c>
       <c r="R14" s="3" t="s">
-        <v>12</v>
+        <v>78</v>
       </c>
       <c r="S14" s="3" t="s">
         <v>12</v>
@@ -1430,13 +1554,13 @@
         <v>12</v>
       </c>
       <c r="P15" s="3" t="s">
-        <v>12</v>
+        <v>53</v>
       </c>
       <c r="Q15" s="3" t="s">
-        <v>12</v>
+        <v>66</v>
       </c>
       <c r="R15" s="3" t="s">
-        <v>12</v>
+        <v>79</v>
       </c>
       <c r="S15" s="3" t="s">
         <v>12</v>
@@ -1490,13 +1614,13 @@
         <v>12</v>
       </c>
       <c r="P16" s="3" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="Q16" s="3" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="R16" s="3" t="s">
-        <v>12</v>
+        <v>80</v>
       </c>
       <c r="S16" s="3" t="s">
         <v>12</v>
@@ -1550,13 +1674,13 @@
         <v>12</v>
       </c>
       <c r="P17" s="3" t="s">
-        <v>12</v>
+        <v>55</v>
       </c>
       <c r="Q17" s="3" t="s">
-        <v>12</v>
+        <v>68</v>
       </c>
       <c r="R17" s="3" t="s">
-        <v>12</v>
+        <v>81</v>
       </c>
       <c r="S17" s="3" t="s">
         <v>12</v>
@@ -1610,13 +1734,13 @@
         <v>12</v>
       </c>
       <c r="P18" s="3" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="Q18" s="3" t="s">
-        <v>12</v>
+        <v>69</v>
       </c>
       <c r="R18" s="3" t="s">
-        <v>12</v>
+        <v>82</v>
       </c>
       <c r="S18" s="3" t="s">
         <v>12</v>
@@ -1670,13 +1794,13 @@
         <v>12</v>
       </c>
       <c r="P19" s="3" t="s">
-        <v>12</v>
+        <v>57</v>
       </c>
       <c r="Q19" s="3" t="s">
-        <v>12</v>
+        <v>70</v>
       </c>
       <c r="R19" s="3" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="S19" s="3" t="s">
         <v>12</v>
@@ -1730,13 +1854,13 @@
         <v>12</v>
       </c>
       <c r="P20" s="3" t="s">
-        <v>12</v>
+        <v>58</v>
       </c>
       <c r="Q20" s="3" t="s">
-        <v>12</v>
+        <v>71</v>
       </c>
       <c r="R20" s="3" t="s">
-        <v>12</v>
+        <v>84</v>
       </c>
       <c r="S20" s="3" t="s">
         <v>12</v>
@@ -1762,6 +1886,7 @@
     <mergeCell ref="E5:O5"/>
     <mergeCell ref="P5:Z5"/>
   </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
geom dont change method
</commit_message>
<xml_diff>
--- a/ExcelData/table.xlsx
+++ b/ExcelData/table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NULS\Desktop\StarAutomation\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7AAB8F2-F1AD-46E2-88DD-C9E38D41D805}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58D186D2-B3E9-4375-9974-8C8936E8B1B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27540" yWindow="1545" windowWidth="21135" windowHeight="11220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4575" yWindow="2445" windowWidth="20310" windowHeight="11820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="87">
   <si>
     <t>Ядро запуска задачи</t>
   </si>
@@ -360,6 +360,9 @@
   </si>
   <si>
     <t>0.1</t>
+  </si>
+  <si>
+    <t>0.4</t>
   </si>
 </sst>
 </file>
@@ -935,8 +938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="E4:Z20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H7" workbookViewId="0">
-      <selection activeCell="V10" sqref="V10"/>
+    <sheetView tabSelected="1" topLeftCell="L7" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9:R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1146,7 +1149,7 @@
         <v>72</v>
       </c>
       <c r="S8" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="T8" s="3" t="s">
         <v>85</v>
@@ -1175,25 +1178,25 @@
         <v>1.2</v>
       </c>
       <c r="F9" s="3">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G9" s="3">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H9" s="3">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I9" s="3">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J9" s="3">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K9" s="3">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L9" s="3">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M9" s="6"/>
       <c r="N9" s="3" t="s">
@@ -1221,7 +1224,7 @@
         <v>85</v>
       </c>
       <c r="V9" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="W9" s="3" t="s">
         <v>85</v>
@@ -1241,25 +1244,25 @@
         <v>13</v>
       </c>
       <c r="F10" s="3">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G10" s="3">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H10" s="3">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I10" s="3">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J10" s="3">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K10" s="3">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="L10" s="3">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="M10" s="6"/>
       <c r="N10" s="3" t="s">
@@ -1293,7 +1296,7 @@
         <v>85</v>
       </c>
       <c r="X10" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="Y10" s="3" t="s">
         <v>85</v>
@@ -1365,7 +1368,7 @@
         <v>85</v>
       </c>
       <c r="Z11" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="5:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1410,7 +1413,7 @@
         <v>76</v>
       </c>
       <c r="S12" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="T12" s="3" t="s">
         <v>85</v>
@@ -1476,7 +1479,7 @@
         <v>77</v>
       </c>
       <c r="S13" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="T13" s="3" t="s">
         <v>85</v>
@@ -1542,7 +1545,7 @@
         <v>78</v>
       </c>
       <c r="S14" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="T14" s="3" t="s">
         <v>85</v>
@@ -1608,7 +1611,7 @@
         <v>79</v>
       </c>
       <c r="S15" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="T15" s="3" t="s">
         <v>85</v>
@@ -1674,7 +1677,7 @@
         <v>80</v>
       </c>
       <c r="S16" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="T16" s="3" t="s">
         <v>85</v>
@@ -1740,7 +1743,7 @@
         <v>81</v>
       </c>
       <c r="S17" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="T17" s="3" t="s">
         <v>85</v>
@@ -1806,7 +1809,7 @@
         <v>82</v>
       </c>
       <c r="S18" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="T18" s="3" t="s">
         <v>85</v>
@@ -1872,7 +1875,7 @@
         <v>83</v>
       </c>
       <c r="S19" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="T19" s="3" t="s">
         <v>85</v>
@@ -1938,7 +1941,7 @@
         <v>84</v>
       </c>
       <c r="S20" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="T20" s="3" t="s">
         <v>85</v>

</xml_diff>